<commit_message>
edit folder, add diagrams on hotel_booking projects
</commit_message>
<xml_diff>
--- a/payroll_bot/payroll.xlsx
+++ b/payroll_bot/payroll.xlsx
@@ -20,7 +20,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0\ [$₫-42A]_-;\-* #,##0\ [$₫-42A]_-;_-* &quot;-&quot;\ [$₫-42A]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -44,6 +44,12 @@
       <sz val="14"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -59,7 +65,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -270,6 +276,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -290,6 +311,19 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -339,6 +373,19 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -391,6 +438,17 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -429,6 +487,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -439,6 +517,15 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -447,9 +534,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -460,22 +545,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -484,7 +554,9 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -495,54 +567,40 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -572,7 +630,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -588,7 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -600,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -618,7 +676,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -630,42 +688,72 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,8 +1135,8 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1065,33 +1153,33 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">
-      <c r="A1" s="50" t="inlineStr">
+      <c r="A1" s="46" t="inlineStr">
         <is>
           <t>T9</t>
         </is>
       </c>
-      <c r="B1" s="40" t="inlineStr">
+      <c r="B1" s="45" t="inlineStr">
         <is>
           <t>Trợ giảng</t>
         </is>
       </c>
-      <c r="C1" s="41" t="n"/>
-      <c r="D1" s="42" t="n"/>
-      <c r="E1" s="40" t="inlineStr">
+      <c r="C1" s="53" t="n"/>
+      <c r="D1" s="54" t="n"/>
+      <c r="E1" s="45" t="inlineStr">
         <is>
           <t>Phụ đạo</t>
         </is>
       </c>
-      <c r="F1" s="41" t="n"/>
-      <c r="G1" s="42" t="n"/>
-      <c r="H1" s="45" t="inlineStr">
+      <c r="F1" s="53" t="n"/>
+      <c r="G1" s="54" t="n"/>
+      <c r="H1" s="55" t="inlineStr">
         <is>
           <t>Gia sư</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15" customFormat="1" customHeight="1" s="1" thickBot="1">
-      <c r="A2" s="51" t="n"/>
+      <c r="A2" s="56" t="n"/>
       <c r="B2" s="15" t="inlineStr">
         <is>
           <t>Lớp</t>
@@ -1122,7 +1210,7 @@
           <t>Lương</t>
         </is>
       </c>
-      <c r="H2" s="46" t="n"/>
+      <c r="H2" s="57" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
@@ -1236,8 +1324,14 @@
       <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="n"/>
-      <c r="C9" s="18" t="n"/>
+      <c r="B9" s="18" t="inlineStr">
+        <is>
+          <t>HC9.1</t>
+        </is>
+      </c>
+      <c r="C9" s="18" t="n">
+        <v>9</v>
+      </c>
       <c r="D9" s="7">
         <f>IF(AND(C9&gt;0,C9&lt;13),120000,IF(AND(C9&gt;12,C9&lt;18),140000,IF(AND(C9&gt;17,C9&lt;23),160000,IF(AND(C9&gt;22,C9&lt;28),180000,IF(AND(C9&gt;26,C9&lt;32),200000,IF(C9&gt;31,220000,0))))))</f>
         <v/>
@@ -1260,8 +1354,14 @@
         <f>IF(AND(C10&gt;0,C10&lt;13),120000,IF(AND(C10&gt;12,C10&lt;18),140000,IF(AND(C10&gt;17,C10&lt;23),160000,IF(AND(C10&gt;22,C10&lt;28),180000,IF(AND(C10&gt;26,C10&lt;32),200000,IF(C10&gt;31,220000,0))))))</f>
         <v/>
       </c>
-      <c r="E10" s="28" t="n"/>
-      <c r="F10" s="22" t="n"/>
+      <c r="E10" s="28" t="inlineStr">
+        <is>
+          <t>18:00-20:30</t>
+        </is>
+      </c>
+      <c r="F10" s="22" t="n">
+        <v>2.5</v>
+      </c>
       <c r="G10" s="33">
         <f>F10*60000</f>
         <v/>
@@ -1278,8 +1378,14 @@
         <f>IF(AND(C11&gt;0,C11&lt;13),120000,IF(AND(C11&gt;12,C11&lt;18),140000,IF(AND(C11&gt;17,C11&lt;23),160000,IF(AND(C11&gt;22,C11&lt;28),180000,IF(AND(C11&gt;26,C11&lt;32),200000,IF(C11&gt;31,220000,0))))))</f>
         <v/>
       </c>
-      <c r="E11" s="28" t="n"/>
-      <c r="F11" s="22" t="n"/>
+      <c r="E11" s="28" t="inlineStr">
+        <is>
+          <t>14:00-16:30</t>
+        </is>
+      </c>
+      <c r="F11" s="22" t="n">
+        <v>2.5</v>
+      </c>
       <c r="G11" s="33">
         <f>F11*60000</f>
         <v/>
@@ -1296,8 +1402,14 @@
         <f>IF(AND(C12&gt;0,C12&lt;13),120000,IF(AND(C12&gt;12,C12&lt;18),140000,IF(AND(C12&gt;17,C12&lt;23),160000,IF(AND(C12&gt;22,C12&lt;28),180000,IF(AND(C12&gt;26,C12&lt;32),200000,IF(C12&gt;31,220000,0))))))</f>
         <v/>
       </c>
-      <c r="E12" s="28" t="n"/>
-      <c r="F12" s="22" t="n"/>
+      <c r="E12" s="28" t="inlineStr">
+        <is>
+          <t>14:00-16:30</t>
+        </is>
+      </c>
+      <c r="F12" s="22" t="n">
+        <v>2.5</v>
+      </c>
       <c r="G12" s="33">
         <f>F12*60000</f>
         <v/>
@@ -1310,8 +1422,14 @@
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="18" t="n"/>
-      <c r="C13" s="18" t="n"/>
+      <c r="B13" s="18" t="inlineStr">
+        <is>
+          <t>TC7.0A</t>
+        </is>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>22</v>
+      </c>
       <c r="D13" s="7">
         <f>IF(AND(C13&gt;0,C13&lt;13),120000,IF(AND(C13&gt;12,C13&lt;18),140000,IF(AND(C13&gt;17,C13&lt;23),160000,IF(AND(C13&gt;22,C13&lt;28),180000,IF(AND(C13&gt;26,C13&lt;32),200000,IF(C13&gt;31,220000,0))))))</f>
         <v/>
@@ -1364,8 +1482,14 @@
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="n"/>
-      <c r="C16" s="18" t="n"/>
+      <c r="B16" s="18" t="inlineStr">
+        <is>
+          <t>HC9.1</t>
+        </is>
+      </c>
+      <c r="C16" s="18" t="n">
+        <v>9</v>
+      </c>
       <c r="D16" s="7">
         <f>IF(AND(C16&gt;0,C16&lt;13),120000,IF(AND(C16&gt;12,C16&lt;18),140000,IF(AND(C16&gt;17,C16&lt;23),160000,IF(AND(C16&gt;22,C16&lt;28),180000,IF(AND(C16&gt;26,C16&lt;32),200000,IF(C16&gt;31,220000,0))))))</f>
         <v/>
@@ -1388,8 +1512,14 @@
         <f>IF(AND(C17&gt;0,C17&lt;13),120000,IF(AND(C17&gt;12,C17&lt;18),140000,IF(AND(C17&gt;17,C17&lt;23),160000,IF(AND(C17&gt;22,C17&lt;28),180000,IF(AND(C17&gt;26,C17&lt;32),200000,IF(C17&gt;31,220000,0))))))</f>
         <v/>
       </c>
-      <c r="E17" s="28" t="n"/>
-      <c r="F17" s="22" t="n"/>
+      <c r="E17" s="28" t="inlineStr">
+        <is>
+          <t>18:00-20:00</t>
+        </is>
+      </c>
+      <c r="F17" s="22" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="33">
         <f>F17*60000</f>
         <v/>
@@ -1406,8 +1536,14 @@
         <f>IF(AND(C18&gt;0,C18&lt;13),120000,IF(AND(C18&gt;12,C18&lt;18),140000,IF(AND(C18&gt;17,C18&lt;23),160000,IF(AND(C18&gt;22,C18&lt;28),180000,IF(AND(C18&gt;26,C18&lt;32),200000,IF(C18&gt;31,220000,0))))))</f>
         <v/>
       </c>
-      <c r="E18" s="28" t="n"/>
-      <c r="F18" s="22" t="n"/>
+      <c r="E18" s="28" t="inlineStr">
+        <is>
+          <t>14:00-16:30</t>
+        </is>
+      </c>
+      <c r="F18" s="22" t="n">
+        <v>2.5</v>
+      </c>
       <c r="G18" s="33">
         <f>F18*60000</f>
         <v/>
@@ -1418,29 +1554,19 @@
       <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="18" t="inlineStr">
-        <is>
-          <t>HC9.1</t>
-        </is>
-      </c>
-      <c r="C19" s="18" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
+      <c r="B19" s="18" t="n"/>
+      <c r="C19" s="18" t="n"/>
       <c r="D19" s="7">
         <f>IF(AND(C19&gt;0,C19&lt;13),120000,IF(AND(C19&gt;12,C19&lt;18),140000,IF(AND(C19&gt;17,C19&lt;23),160000,IF(AND(C19&gt;22,C19&lt;28),180000,IF(AND(C19&gt;26,C19&lt;32),200000,IF(C19&gt;31,220000,0))))))</f>
         <v/>
       </c>
       <c r="E19" s="28" t="inlineStr">
         <is>
-          <t>HC9.1</t>
-        </is>
-      </c>
-      <c r="F19" s="22" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+          <t>14:00-16:30</t>
+        </is>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>2.5</v>
       </c>
       <c r="G19" s="33">
         <f>F19*60000</f>
@@ -1454,8 +1580,14 @@
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="n"/>
-      <c r="C20" s="18" t="n"/>
+      <c r="B20" s="18" t="inlineStr">
+        <is>
+          <t>TC7.0A</t>
+        </is>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>22</v>
+      </c>
       <c r="D20" s="7">
         <f>IF(AND(C20&gt;0,C20&lt;13),120000,IF(AND(C20&gt;12,C20&lt;18),140000,IF(AND(C20&gt;17,C20&lt;23),160000,IF(AND(C20&gt;22,C20&lt;28),180000,IF(AND(C20&gt;26,C20&lt;32),200000,IF(C20&gt;31,220000,0))))))</f>
         <v/>
@@ -1490,8 +1622,16 @@
       <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="18" t="n"/>
-      <c r="C22" s="18" t="n"/>
+      <c r="B22" s="18" t="inlineStr">
+        <is>
+          <t>HC9.1</t>
+        </is>
+      </c>
+      <c r="C22" s="18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="D22" s="7">
         <f>IF(AND(C22&gt;0,C22&lt;13),120000,IF(AND(C22&gt;12,C22&lt;18),140000,IF(AND(C22&gt;17,C22&lt;23),160000,IF(AND(C22&gt;22,C22&lt;28),180000,IF(AND(C22&gt;26,C22&lt;32),200000,IF(C22&gt;31,220000,0))))))</f>
         <v/>
@@ -1685,7 +1825,7 @@
       <c r="H32" s="38" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="43" t="inlineStr">
+      <c r="A33" s="51" t="inlineStr">
         <is>
           <t>Tổng</t>
         </is>
@@ -1708,17 +1848,17 @@
       </c>
     </row>
     <row r="34" ht="19" customHeight="1" thickBot="1">
-      <c r="A34" s="44" t="n"/>
-      <c r="B34" s="47">
+      <c r="A34" s="58" t="n"/>
+      <c r="B34" s="59">
         <f>SUM(D33,G33, H33)</f>
         <v/>
       </c>
-      <c r="C34" s="48" t="n"/>
-      <c r="D34" s="48" t="n"/>
-      <c r="E34" s="48" t="n"/>
-      <c r="F34" s="48" t="n"/>
-      <c r="G34" s="48" t="n"/>
-      <c r="H34" s="49" t="n"/>
+      <c r="C34" s="60" t="n"/>
+      <c r="D34" s="60" t="n"/>
+      <c r="E34" s="60" t="n"/>
+      <c r="F34" s="60" t="n"/>
+      <c r="G34" s="60" t="n"/>
+      <c r="H34" s="61" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1754,12 +1894,12 @@
   <sheetData>
     <row r="3" ht="15" customHeight="1" thickBot="1"/>
     <row r="4" ht="15" customHeight="1" thickBot="1">
-      <c r="C4" s="43" t="inlineStr">
+      <c r="C4" s="51" t="inlineStr">
         <is>
           <t>CÁCH TÍNH LƯƠNG</t>
         </is>
       </c>
-      <c r="D4" s="52" t="n"/>
+      <c r="D4" s="62" t="n"/>
     </row>
     <row r="5">
       <c r="C5" s="11" t="inlineStr">

</xml_diff>